<commit_message>
Mise a jour du fichier statistique.xlsx
</commit_message>
<xml_diff>
--- a/Fichiers/statistiques.xlsx
+++ b/Fichiers/statistiques.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Nom-equipe</t>
   </si>
@@ -70,28 +70,55 @@
     <t xml:space="preserve">Remplacement</t>
   </si>
   <si>
+    <t xml:space="preserve">images</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chelsea</t>
   </si>
   <si>
+    <t xml:space="preserve">../images/chelsea.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barcelona</t>
   </si>
   <si>
+    <t xml:space="preserve">../images/barca.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Juventus</t>
   </si>
   <si>
+    <t xml:space="preserve">../images/juventus.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marseille</t>
   </si>
   <si>
+    <t xml:space="preserve">../images/marseille.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">PSG</t>
   </si>
   <si>
+    <t xml:space="preserve">../images/psg.jpeg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bayern</t>
   </si>
   <si>
+    <t xml:space="preserve">../images/bayern.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dortmund</t>
   </si>
   <si>
+    <t xml:space="preserve">../images/dortmund.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Monaco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../images/monaco.png</t>
   </si>
 </sst>
 </file>
@@ -196,10 +223,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q8" activeCellId="0" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -214,7 +241,8 @@
     <col collapsed="false" hidden="false" max="14" min="9" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3622448979592"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="14.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="24.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -266,10 +294,13 @@
       <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -316,10 +347,13 @@
       <c r="P2" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="Q2" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -366,10 +400,13 @@
       <c r="P3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="Q3" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
@@ -416,10 +453,13 @@
       <c r="P4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="Q4" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
@@ -466,10 +506,13 @@
       <c r="P5" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="Q5" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3</v>
@@ -516,10 +559,13 @@
       <c r="P6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="Q6" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>3</v>
@@ -566,10 +612,13 @@
       <c r="P7" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="Q7" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>4</v>
@@ -616,10 +665,13 @@
       <c r="P8" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="Q8" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>4</v>
@@ -665,6 +717,9 @@
       </c>
       <c r="P9" s="0" t="n">
         <v>5</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>